<commit_message>
Refactor Code and Add Documentation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,35 +476,75 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021-11-18</t>
+          <t>2021-11-23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19:33:00</t>
+          <t>11:17:47</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bayar Cicilan</t>
+          <t>Top Up From BCA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Transfer</t>
+          <t>Top Up</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>10000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>YunusMars</t>
+          <t>BCA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>MichaelH</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2021-11-23</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11:18:03</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Top Up From BCA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Top Up</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>BCA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>MichaelH</t>
         </is>

</xml_diff>